<commit_message>
Update planted column load to 250kN
- Update `structural_design.py` CONST dictionary `PLANTED_P` to 250.0.
- Regenerate `My Drawing_ANALYTICAL.dxf` and `My Drawing_CALCS.xlsx`.
- Fix syntax error in import statement.
</commit_message>
<xml_diff>
--- a/My Drawing_CALCS.xlsx
+++ b/My Drawing_CALCS.xlsx
@@ -484,17 +484,17 @@
         <v>0.4</v>
       </c>
       <c r="D2" t="n">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="n">
-        <v>502</v>
+        <v>290</v>
       </c>
       <c r="F2" t="n">
-        <v>354</v>
+        <v>212</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>13 T16</t>
+          <t>10 T16</t>
         </is>
       </c>
     </row>
@@ -541,14 +541,14 @@
         <v>0.4</v>
       </c>
       <c r="E4" t="n">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="F4" t="n">
-        <v>325</v>
+        <v>185</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>7 T16</t>
+          <t>4 T16</t>
         </is>
       </c>
     </row>
@@ -619,17 +619,17 @@
         <v>0.4</v>
       </c>
       <c r="D7" t="n">
-        <v>0.55</v>
+        <v>0.45</v>
       </c>
       <c r="E7" t="n">
-        <v>438</v>
+        <v>252</v>
       </c>
       <c r="F7" t="n">
-        <v>349</v>
+        <v>207</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>13 T16</t>
+          <t>10 T16</t>
         </is>
       </c>
     </row>
@@ -646,17 +646,17 @@
         <v>0.4</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E8" t="n">
-        <v>293</v>
+        <v>167</v>
       </c>
       <c r="F8" t="n">
-        <v>337</v>
+        <v>196</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10 T16</t>
+          <t>7 T16</t>
         </is>
       </c>
     </row>
@@ -676,14 +676,14 @@
         <v>0.4</v>
       </c>
       <c r="E9" t="n">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="F9" t="n">
-        <v>324</v>
+        <v>184</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>6 T16</t>
+          <t>3 T16</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
         <v>0.4</v>
       </c>
       <c r="D13" t="n">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="E13" t="n">
-        <v>685</v>
+        <v>401</v>
       </c>
       <c r="F13" t="n">
-        <v>370</v>
+        <v>226</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>15 T16</t>
+          <t>12 T16</t>
         </is>
       </c>
     </row>
@@ -1027,14 +1027,14 @@
         <v>0.4</v>
       </c>
       <c r="E22" t="n">
-        <v>185</v>
+        <v>104</v>
       </c>
       <c r="F22" t="n">
-        <v>328</v>
+        <v>188</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>8 T16</t>
+          <t>5 T16</t>
         </is>
       </c>
     </row>
@@ -1051,17 +1051,17 @@
         <v>0.4</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E23" t="n">
-        <v>344</v>
+        <v>196</v>
       </c>
       <c r="F23" t="n">
-        <v>341</v>
+        <v>200</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>12 T16</t>
+          <t>9 T16</t>
         </is>
       </c>
     </row>
@@ -1243,14 +1243,14 @@
         <v>0.4</v>
       </c>
       <c r="E30" t="n">
-        <v>185</v>
+        <v>104</v>
       </c>
       <c r="F30" t="n">
-        <v>328</v>
+        <v>188</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>8 T16</t>
+          <t>5 T16</t>
         </is>
       </c>
     </row>
@@ -1267,17 +1267,17 @@
         <v>0.4</v>
       </c>
       <c r="D31" t="n">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="E31" t="n">
-        <v>685</v>
+        <v>401</v>
       </c>
       <c r="F31" t="n">
-        <v>370</v>
+        <v>226</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>15 T16</t>
+          <t>12 T16</t>
         </is>
       </c>
     </row>
@@ -1294,17 +1294,17 @@
         <v>0.4</v>
       </c>
       <c r="D32" t="n">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="E32" t="n">
-        <v>501</v>
+        <v>290</v>
       </c>
       <c r="F32" t="n">
-        <v>354</v>
+        <v>212</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>13 T16</t>
+          <t>10 T16</t>
         </is>
       </c>
     </row>
@@ -1699,17 +1699,17 @@
         <v>0.4</v>
       </c>
       <c r="D47" t="n">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="E47" t="n">
-        <v>509</v>
+        <v>295</v>
       </c>
       <c r="F47" t="n">
-        <v>355</v>
+        <v>213</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>13 T16</t>
+          <t>10 T16</t>
         </is>
       </c>
     </row>
@@ -1726,17 +1726,17 @@
         <v>0.4</v>
       </c>
       <c r="D48" t="n">
-        <v>0.55</v>
+        <v>0.4</v>
       </c>
       <c r="E48" t="n">
-        <v>370</v>
+        <v>212</v>
       </c>
       <c r="F48" t="n">
-        <v>344</v>
+        <v>202</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>11 T16</t>
+          <t>9 T16</t>
         </is>
       </c>
     </row>
@@ -1753,17 +1753,17 @@
         <v>0.4</v>
       </c>
       <c r="D49" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E49" t="n">
-        <v>294</v>
+        <v>167</v>
       </c>
       <c r="F49" t="n">
-        <v>337</v>
+        <v>196</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>10 T16</t>
+          <t>8 T16</t>
         </is>
       </c>
     </row>
@@ -1783,14 +1783,14 @@
         <v>0.4</v>
       </c>
       <c r="E50" t="n">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="F50" t="n">
-        <v>324</v>
+        <v>184</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>6 T16</t>
+          <t>3 T16</t>
         </is>
       </c>
     </row>
@@ -1807,17 +1807,17 @@
         <v>0.4</v>
       </c>
       <c r="D51" t="n">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="E51" t="n">
-        <v>466</v>
+        <v>269</v>
       </c>
       <c r="F51" t="n">
-        <v>351</v>
+        <v>209</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>12 T16</t>
+          <t>10 T16</t>
         </is>
       </c>
     </row>
@@ -1834,17 +1834,17 @@
         <v>0.4</v>
       </c>
       <c r="D52" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="E52" t="n">
-        <v>592</v>
+        <v>344</v>
       </c>
       <c r="F52" t="n">
-        <v>362</v>
+        <v>219</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>14 T16</t>
+          <t>12 T16</t>
         </is>
       </c>
     </row>
@@ -1888,17 +1888,17 @@
         <v>0.4</v>
       </c>
       <c r="D54" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="E54" t="n">
-        <v>592</v>
+        <v>344</v>
       </c>
       <c r="F54" t="n">
-        <v>362</v>
+        <v>219</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>14 T16</t>
+          <t>12 T16</t>
         </is>
       </c>
     </row>
@@ -1915,17 +1915,17 @@
         <v>0.4</v>
       </c>
       <c r="D55" t="n">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="E55" t="n">
-        <v>466</v>
+        <v>269</v>
       </c>
       <c r="F55" t="n">
-        <v>351</v>
+        <v>209</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>12 T16</t>
+          <t>10 T16</t>
         </is>
       </c>
     </row>
@@ -1942,17 +1942,17 @@
         <v>0.4</v>
       </c>
       <c r="D56" t="n">
-        <v>0.55</v>
+        <v>0.4</v>
       </c>
       <c r="E56" t="n">
-        <v>370</v>
+        <v>212</v>
       </c>
       <c r="F56" t="n">
-        <v>344</v>
+        <v>202</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>11 T16</t>
+          <t>9 T16</t>
         </is>
       </c>
     </row>
@@ -1969,17 +1969,17 @@
         <v>0.4</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E57" t="n">
-        <v>361</v>
+        <v>207</v>
       </c>
       <c r="F57" t="n">
-        <v>342</v>
+        <v>201</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>12 T16</t>
+          <t>9 T16</t>
         </is>
       </c>
     </row>
@@ -1996,17 +1996,17 @@
         <v>0.4</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E58" t="n">
-        <v>361</v>
+        <v>207</v>
       </c>
       <c r="F58" t="n">
-        <v>342</v>
+        <v>201</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>12 T16</t>
+          <t>9 T16</t>
         </is>
       </c>
     </row>

</xml_diff>